<commit_message>
implemented spectral and hierarchical clustering
</commit_message>
<xml_diff>
--- a/metrics.xlsx
+++ b/metrics.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>silhouette</t>
   </si>
@@ -28,13 +28,10 @@
     <t>Iteration name</t>
   </si>
   <si>
-    <t>tamere</t>
-  </si>
-  <si>
-    <t>stppp</t>
-  </si>
-  <si>
-    <t>trrr</t>
+    <t>kmeans 1</t>
+  </si>
+  <si>
+    <t>dbscan 1</t>
   </si>
 </sst>
 </file>
@@ -392,7 +389,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -420,13 +417,13 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>-0.4546614108580692</v>
+        <v>0.4618231593530843</v>
       </c>
       <c r="C2">
-        <v>0.3630617322335979</v>
+        <v>921165.0807396912</v>
       </c>
       <c r="D2">
-        <v>7.031098165599168</v>
+        <v>0.8172181159728882</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -434,27 +431,13 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>0.4618231593530843</v>
+        <v>-0.4546614108580692</v>
       </c>
       <c r="C3">
-        <v>921165.0807396912</v>
+        <v>0.3630617322335979</v>
       </c>
       <c r="D3">
-        <v>0.8172181159728882</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4">
-        <v>0.4618231593530843</v>
-      </c>
-      <c r="C4">
-        <v>921165.0807396912</v>
-      </c>
-      <c r="D4">
-        <v>0.8172181159728882</v>
+        <v>7.031098165599168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tuning kmeans for iter 1
</commit_message>
<xml_diff>
--- a/metrics.xlsx
+++ b/metrics.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>silhouette</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t>dbscan 1</t>
+  </si>
+  <si>
+    <t>kmeans_tuning_1</t>
   </si>
 </sst>
 </file>
@@ -389,7 +392,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -440,6 +443,20 @@
         <v>7.031098165599168</v>
       </c>
     </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>0.5050436415844799</v>
+      </c>
+      <c r="C4">
+        <v>714477.0893068067</v>
+      </c>
+      <c r="D4">
+        <v>0.4315535954435768</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Refacto spectral and hierarchical
</commit_message>
<xml_diff>
--- a/metrics.xlsx
+++ b/metrics.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>silhouette</t>
   </si>
@@ -35,6 +35,12 @@
   </si>
   <si>
     <t>kmeans_tuning_1</t>
+  </si>
+  <si>
+    <t>spectral_1</t>
+  </si>
+  <si>
+    <t>hierarchical_1</t>
   </si>
 </sst>
 </file>
@@ -392,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -457,6 +463,34 @@
         <v>0.4315535954435768</v>
       </c>
     </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>-0.3862637995641255</v>
+      </c>
+      <c r="C5">
+        <v>0.4725908679043076</v>
+      </c>
+      <c r="D5">
+        <v>4.155297896218482</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>0.9939182672879472</v>
+      </c>
+      <c r="C6">
+        <v>36211.61359472208</v>
+      </c>
+      <c r="D6">
+        <v>0.2206786182786379</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>